<commit_message>
Added Images for Home Page, create commoncomponents for navbar and footer and added AntD library
</commit_message>
<xml_diff>
--- a/public/excel_files/Static_data.xlsx
+++ b/public/excel_files/Static_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAURANG\OneDrive\Desktop\Ecompusell-printer-website\ecompusell\public\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8722FEB-0315-45E3-A62A-E67C00430E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16517074-2EE6-4256-BE93-94C6F32F3E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,13 +397,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>

</xml_diff>